<commit_message>
Small tweaks in error handling
</commit_message>
<xml_diff>
--- a/articles.xlsx
+++ b/articles.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1052,6 +1052,26 @@
         <v>2</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>50 najbardziej ekscytujących nastolatków w światowym futbolu wg FourFourTwo</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Dwóch piłkarzy Blaugrany w rankingu</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>http://fcbarca.com/108084-50-najbardziej-ekscytujacych-nastolatkow-w-swiatowym-futbolu-wg-fourfourtwo.html</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Change to DB connectio,  is more efficient
</commit_message>
<xml_diff>
--- a/articles.xlsx
+++ b/articles.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1072,6 +1072,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Deadly storm slams into California's coast</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>The storm is expected to bring deadly flooding, landsides, and power outages affecting millions.</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>https://bbc.co.uk/news/world-us-canada-64169954</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Now doesnt duplicate articles
</commit_message>
<xml_diff>
--- a/articles.xlsx
+++ b/articles.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1092,6 +1092,26 @@
         <v>2</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Pedri: Mam jeszcze wiele do poprawy</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>20-letni pomocnik w wywiadzie dla DAZN</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>http://fcbarca.com/108091-pedri-mam-jeszcze-wiele-do-poprawy.html</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>